<commit_message>
Rebalanced armor, started working on new map
</commit_message>
<xml_diff>
--- a/Untitled-RPG/Assets/Excel/Equipment Balancing.xlsx
+++ b/Untitled-RPG/Assets/Excel/Equipment Balancing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Untitled-RPG\Untitled-RPG\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1045608A-9F9A-4ABA-9A40-83B6076EC57C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92F37E9-CAF3-47BA-8B82-4A6B871D60D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9315256A-FBE0-4846-A7B0-BE8037A06B15}"/>
+    <workbookView xWindow="28680" yWindow="-9120" windowWidth="16440" windowHeight="29040" xr2:uid="{9315256A-FBE0-4846-A7B0-BE8037A06B15}"/>
   </bookViews>
   <sheets>
     <sheet name="Equipment" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
   <si>
     <t>Stamina</t>
   </si>
@@ -94,9 +94,6 @@
     <t>AttacksValue</t>
   </si>
   <si>
-    <t>HealthStaminaValue</t>
-  </si>
-  <si>
     <t>StatsValue</t>
   </si>
   <si>
@@ -185,6 +182,18 @@
   </si>
   <si>
     <t>CritBlockValue</t>
+  </si>
+  <si>
+    <t>DefenseValue</t>
+  </si>
+  <si>
+    <t>StaminaValue</t>
+  </si>
+  <si>
+    <t>HealthValue</t>
+  </si>
+  <si>
+    <t>Armor (reference chest below)</t>
   </si>
 </sst>
 </file>
@@ -330,7 +339,147 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="65">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBA8BDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5757"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBA8BDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5757"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBA8BDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5757"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBA8BDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5757"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -965,13 +1114,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B67F58F-2800-4B7E-AC83-84187933C49D}">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H21" sqref="H21"/>
+      <selection pane="bottomRight" activeCell="P37" sqref="P37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,14 +1137,19 @@
     <col min="10" max="10" width="12.5703125" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
     <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" customWidth="1"/>
+    <col min="17" max="18" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
@@ -1003,89 +1157,126 @@
       <c r="F1" s="22"/>
       <c r="G1" s="15"/>
       <c r="H1" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I1" s="22"/>
       <c r="J1" s="22"/>
       <c r="K1" s="22"/>
       <c r="L1" s="22"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N1" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>26</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>27</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>28</v>
       </c>
-      <c r="F2" t="s">
-        <v>29</v>
-      </c>
       <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
         <v>25</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>26</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>28</v>
       </c>
-      <c r="L2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="10">
+        <v>50</v>
+      </c>
+      <c r="C4" s="10">
         <v>100</v>
       </c>
-      <c r="C4" s="10">
-        <v>150</v>
-      </c>
       <c r="D4" s="10">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="E4" s="10">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="F4" s="10">
-        <v>700</v>
+        <v>760</v>
       </c>
       <c r="H4" s="10">
-        <f>B4*Variables!$B$18</f>
+        <f>B4*Variables!$B$20</f>
+        <v>92.5</v>
+      </c>
+      <c r="I4" s="10">
+        <f>C4*Variables!$B$20</f>
         <v>185</v>
       </c>
-      <c r="I4" s="10">
-        <f>C4*Variables!$B$18</f>
-        <v>277.5</v>
-      </c>
       <c r="J4" s="10">
-        <f>D4*Variables!$B$18</f>
-        <v>462.5</v>
+        <f>D4*Variables!$B$20</f>
+        <v>370</v>
       </c>
       <c r="K4" s="10">
-        <f>E4*Variables!$B$18</f>
-        <v>925</v>
+        <f>E4*Variables!$B$20</f>
+        <v>740</v>
       </c>
       <c r="L4" s="10">
-        <f>F4*Variables!$B$18</f>
-        <v>1295</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <f>F4*Variables!$B$20</f>
+        <v>1406</v>
+      </c>
+      <c r="N4" s="10">
+        <v>0</v>
+      </c>
+      <c r="O4" s="10">
+        <v>0</v>
+      </c>
+      <c r="P4" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="10">
+        <v>0</v>
+      </c>
+      <c r="R4" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1099,33 +1290,48 @@
         <v>0</v>
       </c>
       <c r="E5" s="10">
+        <v>100</v>
+      </c>
+      <c r="F5" s="10">
         <v>200</v>
       </c>
-      <c r="F5" s="10">
-        <v>500</v>
-      </c>
       <c r="H5" s="10">
-        <f>B5*Variables!$B$18</f>
+        <f>B5*Variables!$B$20</f>
         <v>0</v>
       </c>
       <c r="I5" s="10">
-        <f>C5*Variables!$B$18</f>
+        <f>C5*Variables!$B$20</f>
         <v>0</v>
       </c>
       <c r="J5" s="10">
-        <f>D5*Variables!$B$18</f>
+        <f>D5*Variables!$B$20</f>
         <v>0</v>
       </c>
       <c r="K5" s="10">
-        <f>E5*Variables!$B$18</f>
+        <f>E5*Variables!$B$20</f>
+        <v>185</v>
+      </c>
+      <c r="L5" s="10">
+        <f>F5*Variables!$B$20</f>
         <v>370</v>
       </c>
-      <c r="L5" s="10">
-        <f>F5*Variables!$B$18</f>
-        <v>925</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N5" s="10">
+        <v>0</v>
+      </c>
+      <c r="O5" s="10">
+        <v>0</v>
+      </c>
+      <c r="P5" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="10">
+        <v>0</v>
+      </c>
+      <c r="R5" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1139,33 +1345,48 @@
         <v>0</v>
       </c>
       <c r="E6" s="10">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F6" s="10">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="H6" s="10">
-        <f>B6*Variables!$B$18</f>
+        <f>B6*Variables!$B$20</f>
         <v>0</v>
       </c>
       <c r="I6" s="10">
-        <f>C6*Variables!$B$18</f>
+        <f>C6*Variables!$B$20</f>
         <v>0</v>
       </c>
       <c r="J6" s="10">
-        <f>D6*Variables!$B$18</f>
+        <f>D6*Variables!$B$20</f>
         <v>0</v>
       </c>
       <c r="K6" s="10">
-        <f>E6*Variables!$B$18</f>
-        <v>185</v>
+        <f>E6*Variables!$B$20</f>
+        <v>0</v>
       </c>
       <c r="L6" s="10">
-        <f>F6*Variables!$B$18</f>
-        <v>370</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <f>F6*Variables!$B$20</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="10">
+        <v>0</v>
+      </c>
+      <c r="O6" s="10">
+        <v>0</v>
+      </c>
+      <c r="P6" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="10">
+        <v>0</v>
+      </c>
+      <c r="R6" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1185,27 +1406,42 @@
         <v>0</v>
       </c>
       <c r="H7" s="10">
-        <f>B7*Variables!$B$18</f>
+        <f>B7*Variables!$B$20</f>
         <v>0</v>
       </c>
       <c r="I7" s="10">
-        <f>C7*Variables!$B$18</f>
+        <f>C7*Variables!$B$20</f>
         <v>0</v>
       </c>
       <c r="J7" s="10">
-        <f>D7*Variables!$B$18</f>
+        <f>D7*Variables!$B$20</f>
         <v>0</v>
       </c>
       <c r="K7" s="10">
-        <f>E7*Variables!$B$18</f>
+        <f>E7*Variables!$B$20</f>
         <v>0</v>
       </c>
       <c r="L7" s="10">
-        <f>F7*Variables!$B$18</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <f>F7*Variables!$B$20</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="10">
+        <v>0</v>
+      </c>
+      <c r="O7" s="10">
+        <v>0</v>
+      </c>
+      <c r="P7" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="10">
+        <v>0</v>
+      </c>
+      <c r="R7" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1225,30 +1461,45 @@
         <v>0</v>
       </c>
       <c r="H8" s="10">
-        <f>B8*Variables!$B$18</f>
+        <f>B8*Variables!$B$20</f>
         <v>0</v>
       </c>
       <c r="I8" s="10">
-        <f>C8*Variables!$B$18</f>
+        <f>C8*Variables!$B$20</f>
         <v>0</v>
       </c>
       <c r="J8" s="10">
-        <f>D8*Variables!$B$18</f>
+        <f>D8*Variables!$B$20</f>
         <v>0</v>
       </c>
       <c r="K8" s="10">
-        <f>E8*Variables!$B$18</f>
+        <f>E8*Variables!$B$20</f>
         <v>0</v>
       </c>
       <c r="L8" s="10">
-        <f>F8*Variables!$B$18</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <f>F8*Variables!$B$20</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="10">
+        <v>200</v>
+      </c>
+      <c r="O8" s="10">
+        <v>350</v>
+      </c>
+      <c r="P8" s="10">
+        <v>700</v>
+      </c>
+      <c r="Q8" s="10">
+        <v>1400</v>
+      </c>
+      <c r="R8" s="10">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9"/>
     </row>
-    <row r="10" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1268,27 +1519,41 @@
         <v>0</v>
       </c>
       <c r="H10" s="10">
-        <f>B10*Variables!$B$18</f>
         <v>0</v>
       </c>
       <c r="I10" s="10">
-        <f>C10*Variables!$B$18</f>
+        <f>C10*Variables!$B$20</f>
         <v>0</v>
       </c>
       <c r="J10" s="10">
-        <f>D10*Variables!$B$18</f>
+        <f>D10*Variables!$B$20</f>
         <v>0</v>
       </c>
       <c r="K10" s="10">
-        <f>E10*Variables!$B$18</f>
+        <f>E10*Variables!$B$20</f>
         <v>0</v>
       </c>
       <c r="L10" s="10">
-        <f>F10*Variables!$B$18</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <f>F10*Variables!$B$20</f>
+        <v>0</v>
+      </c>
+      <c r="N10" s="10">
+        <v>0</v>
+      </c>
+      <c r="O10" s="10">
+        <v>0</v>
+      </c>
+      <c r="P10" s="10">
+        <v>100</v>
+      </c>
+      <c r="Q10" s="10">
+        <v>300</v>
+      </c>
+      <c r="R10" s="10">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1302,116 +1567,160 @@
         <v>0</v>
       </c>
       <c r="E11" s="10">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="F11" s="10">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H11" s="10">
-        <f>B11*Variables!$B$18</f>
         <v>0</v>
       </c>
       <c r="I11" s="10">
-        <f>C11*Variables!$B$18</f>
+        <f>C11*Variables!$B$20</f>
         <v>0</v>
       </c>
       <c r="J11" s="10">
-        <f>D11*Variables!$B$18</f>
+        <f>D11*Variables!$B$20</f>
         <v>0</v>
       </c>
       <c r="K11" s="10">
-        <f>E11*Variables!$B$18</f>
-        <v>92.5</v>
+        <f>E11*Variables!$B$20</f>
+        <v>0</v>
       </c>
       <c r="L11" s="10">
-        <f>F11*Variables!$B$18</f>
-        <v>185</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <f>F11*Variables!$B$20</f>
+        <v>0</v>
+      </c>
+      <c r="N11" s="10">
+        <v>0</v>
+      </c>
+      <c r="O11" s="10">
+        <v>0</v>
+      </c>
+      <c r="P11" s="10">
+        <v>20</v>
+      </c>
+      <c r="Q11" s="10">
+        <v>40</v>
+      </c>
+      <c r="R11" s="10">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12"/>
     </row>
-    <row r="13" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="10">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C13" s="10">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D13" s="10">
         <v>50</v>
       </c>
       <c r="E13" s="10">
+        <v>70</v>
+      </c>
+      <c r="F13" s="10">
         <v>100</v>
       </c>
-      <c r="F13" s="10">
-        <v>250</v>
-      </c>
       <c r="H13" s="10">
-        <f>B13*POWER(Variables!$B$18,1.3)</f>
-        <v>33.374479861323103</v>
+        <f>B13*POWER(Variables!$B$20,1.3)</f>
+        <v>22.249653240882068</v>
       </c>
       <c r="I13" s="10">
-        <f>C13*POWER(Variables!$B$18,1.5)</f>
-        <v>62.906801102901433</v>
+        <f>C13*POWER(Variables!$B$20,1.5)</f>
+        <v>75.488161323481719</v>
       </c>
       <c r="J13" s="10">
-        <f>D13*POWER(Variables!$B$18,1.5)</f>
+        <f>D13*POWER(Variables!$B$20,1.5)</f>
         <v>125.81360220580287</v>
       </c>
       <c r="K13" s="10">
-        <f>E13*POWER(Variables!$B$18,1.5)</f>
+        <f>E13*POWER(Variables!$B$20,1.5)</f>
+        <v>176.13904308812403</v>
+      </c>
+      <c r="L13" s="10">
+        <f>F13*POWER(Variables!$B$20,1.5)</f>
         <v>251.62720441160573</v>
       </c>
-      <c r="L13" s="10">
-        <f>F13*POWER(Variables!$B$18,1.5)</f>
-        <v>629.06801102901431</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N13" s="10">
+        <v>10</v>
+      </c>
+      <c r="O13" s="10">
+        <v>30</v>
+      </c>
+      <c r="P13" s="10">
+        <v>50</v>
+      </c>
+      <c r="Q13" s="10">
+        <v>70</v>
+      </c>
+      <c r="R13" s="10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="10">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C14" s="10">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D14" s="10">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E14" s="10">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="F14" s="10">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="H14" s="10">
-        <f>B14*POWER(Variables!$B$18,1.5)</f>
-        <v>12.581360220580287</v>
+        <f>B14*POWER(Variables!$B$20,1.5)</f>
+        <v>0</v>
       </c>
       <c r="I14" s="10">
-        <f>C14*POWER(Variables!$B$18,1.5)</f>
-        <v>25.162720441160573</v>
+        <f>C14*POWER(Variables!$B$20,1.5)</f>
+        <v>0</v>
       </c>
       <c r="J14" s="10">
-        <f>D14*POWER(Variables!$B$18,1.5)</f>
-        <v>50.325440882321146</v>
+        <f>D14*POWER(Variables!$B$20,1.5)</f>
+        <v>0</v>
       </c>
       <c r="K14" s="10">
-        <f>E14*POWER(Variables!$B$18,1.5)</f>
-        <v>125.81360220580287</v>
+        <f>E14*POWER(Variables!$B$20,1.5)</f>
+        <v>0</v>
       </c>
       <c r="L14" s="10">
-        <f>F14*POWER(Variables!$B$18,1.5)</f>
-        <v>377.44080661740861</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <f>F14*POWER(Variables!$B$20,1.5)</f>
+        <v>0</v>
+      </c>
+      <c r="N14" s="10">
+        <v>0</v>
+      </c>
+      <c r="O14" s="10">
+        <v>0</v>
+      </c>
+      <c r="P14" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="10">
+        <v>0</v>
+      </c>
+      <c r="R14" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1422,39 +1731,54 @@
         <v>0</v>
       </c>
       <c r="D15" s="10">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E15" s="10">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="F15" s="10">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="H15" s="10">
-        <f>B15*POWER(Variables!$B$18,1.5)</f>
+        <f>B15*POWER(Variables!$B$20,1.5)</f>
         <v>0</v>
       </c>
       <c r="I15" s="10">
-        <f>C15*POWER(Variables!$B$18,1.5)</f>
+        <f>C15*POWER(Variables!$B$20,1.5)</f>
         <v>0</v>
       </c>
       <c r="J15" s="10">
-        <f>D15*POWER(Variables!$B$18,1.5)</f>
-        <v>0</v>
+        <f>D15*POWER(Variables!$B$20,1.5)</f>
+        <v>25.162720441160573</v>
       </c>
       <c r="K15" s="10">
-        <f>E15*POWER(Variables!$B$18,1.5)</f>
-        <v>125.81360220580287</v>
+        <f>E15*POWER(Variables!$B$20,1.5)</f>
+        <v>75.488161323481719</v>
       </c>
       <c r="L15" s="10">
-        <f>F15*POWER(Variables!$B$18,1.5)</f>
-        <v>125.81360220580287</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <f>F15*POWER(Variables!$B$20,1.5)</f>
+        <v>251.62720441160573</v>
+      </c>
+      <c r="N15" s="10">
+        <v>0</v>
+      </c>
+      <c r="O15" s="10">
+        <v>0</v>
+      </c>
+      <c r="P15" s="10">
+        <v>10</v>
+      </c>
+      <c r="Q15" s="10">
+        <v>30</v>
+      </c>
+      <c r="R15" s="10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16"/>
     </row>
-    <row r="17" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1488,8 +1812,23 @@
       <c r="L17" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N17" s="11">
+        <v>0</v>
+      </c>
+      <c r="O17" s="11">
+        <v>0</v>
+      </c>
+      <c r="P17" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="11">
+        <v>0</v>
+      </c>
+      <c r="R17" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1503,7 +1842,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="11">
-        <v>-0.02</v>
+        <v>-0.01</v>
       </c>
       <c r="F18" s="11">
         <v>-0.05</v>
@@ -1523,49 +1862,79 @@
       <c r="L18" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N18" s="11">
+        <v>0</v>
+      </c>
+      <c r="O18" s="11">
+        <v>0</v>
+      </c>
+      <c r="P18" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="11">
+        <v>0</v>
+      </c>
+      <c r="R18" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="11">
+        <v>0</v>
+      </c>
+      <c r="C20" s="11">
+        <v>0</v>
+      </c>
+      <c r="D20" s="11">
+        <v>0</v>
+      </c>
+      <c r="E20" s="11">
+        <v>0</v>
+      </c>
+      <c r="F20" s="11">
+        <v>0</v>
+      </c>
+      <c r="H20" s="11">
+        <v>0</v>
+      </c>
+      <c r="I20" s="11">
+        <v>0</v>
+      </c>
+      <c r="J20" s="11">
+        <v>0</v>
+      </c>
+      <c r="K20" s="11">
+        <v>0</v>
+      </c>
+      <c r="L20" s="11">
+        <v>0</v>
+      </c>
+      <c r="N20" s="11">
+        <v>0</v>
+      </c>
+      <c r="O20" s="11">
+        <v>0</v>
+      </c>
+      <c r="P20" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="11">
+        <v>0</v>
+      </c>
+      <c r="R20" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="11">
-        <v>0</v>
-      </c>
-      <c r="C20" s="11">
-        <v>0</v>
-      </c>
-      <c r="D20" s="11">
-        <v>0</v>
-      </c>
-      <c r="E20" s="11">
-        <v>0</v>
-      </c>
-      <c r="F20" s="11">
-        <v>0</v>
-      </c>
-      <c r="H20" s="11">
-        <v>0</v>
-      </c>
-      <c r="I20" s="11">
-        <v>0</v>
-      </c>
-      <c r="J20" s="11">
-        <v>0</v>
-      </c>
-      <c r="K20" s="11">
-        <v>0</v>
-      </c>
-      <c r="L20" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>48</v>
-      </c>
       <c r="B21" s="11">
         <v>0</v>
       </c>
@@ -1596,8 +1965,23 @@
       <c r="L21" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N21" s="11">
+        <v>0</v>
+      </c>
+      <c r="O21" s="11">
+        <v>0</v>
+      </c>
+      <c r="P21" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="11">
+        <v>0</v>
+      </c>
+      <c r="R21" s="11">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -1631,102 +2015,157 @@
       <c r="L23" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N23" s="10">
+        <v>0</v>
+      </c>
+      <c r="O23" s="10">
+        <v>0</v>
+      </c>
+      <c r="P23" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="10">
+        <v>0</v>
+      </c>
+      <c r="R23" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B26" s="13">
-        <f>SUM(B4:B8)*Variables!$B$1 + SUM(Equipment!B10:B11)*Variables!$B$2 + SUM(Equipment!B13:B15)*Variables!$B$3 + SUM(Equipment!B17:B18)* Variables!$B$4 +Equipment!B23*Variables!$B$5+ VLOOKUP(Equipment!B2,Variables!$A$10:$B$15,2, FALSE)*Variables!$B$7+SUM(B20:B21)*Variables!$B$6</f>
+        <f>SUM(B4:B7)*Variables!$B$1 + B11*Variables!$B$4 +B8*Variables!$B$2+ SUM(Equipment!B10)*Variables!$B$3 + SUM(Equipment!B13:B15)*Variables!$B$5 + SUM(Equipment!B17:B18)* Variables!$B$6 +Equipment!B23*Variables!$B$7+ VLOOKUP(Equipment!B2,Variables!$A$12:$B$17,2, FALSE)*Variables!$B$9+SUM(B20:B21)*Variables!$B$8</f>
         <v>2000</v>
       </c>
       <c r="C26" s="13">
-        <f>SUM(C4:C8)*Variables!$B$1 + SUM(Equipment!C10:C11)*Variables!$B$2 + SUM(Equipment!C13:C15)*Variables!$B$3 + SUM(Equipment!C17:C18)* Variables!$B$4 +Equipment!C23*Variables!$B$5+ VLOOKUP(Equipment!C2,Variables!$A$10:$B$15,2, FALSE)*Variables!$B$7+SUM(C20:C21)*Variables!$B$6</f>
-        <v>5250</v>
+        <f>SUM(C4:C7)*Variables!$B$1 + C11*Variables!$B$4 +C8*Variables!$B$2+ SUM(Equipment!C10)*Variables!$B$3 + SUM(Equipment!C13:C15)*Variables!$B$5 + SUM(Equipment!C17:C18)* Variables!$B$6 +Equipment!C23*Variables!$B$7+ VLOOKUP(Equipment!C2,Variables!$A$12:$B$17,2, FALSE)*Variables!$B$9+SUM(C20:C21)*Variables!$B$8</f>
+        <v>5000</v>
       </c>
       <c r="D26" s="13">
-        <f>SUM(D4:D8)*Variables!$B$1 + SUM(Equipment!D10:D11)*Variables!$B$2 + SUM(Equipment!D13:D15)*Variables!$B$3 + SUM(Equipment!D17:D18)* Variables!$B$4 +Equipment!D23*Variables!$B$5+ VLOOKUP(Equipment!D2,Variables!$A$10:$B$15,2, FALSE)*Variables!$B$7+SUM(D20:D21)*Variables!$B$6</f>
+        <f>SUM(D4:D7)*Variables!$B$1 + D11*Variables!$B$4 +D8*Variables!$B$2+ SUM(Equipment!D10)*Variables!$B$3 + SUM(Equipment!D13:D15)*Variables!$B$5 + SUM(Equipment!D17:D18)* Variables!$B$6 +Equipment!D23*Variables!$B$7+ VLOOKUP(Equipment!D2,Variables!$A$12:$B$17,2, FALSE)*Variables!$B$9+SUM(D20:D21)*Variables!$B$8</f>
         <v>10000</v>
       </c>
       <c r="E26" s="13">
-        <f>SUM(E4:E8)*Variables!$B$1 + SUM(Equipment!E10:E11)*Variables!$B$2 + SUM(Equipment!E13:E15)*Variables!$B$3 + SUM(Equipment!E17:E18)* Variables!$B$4 +Equipment!E23*Variables!$B$5+ VLOOKUP(Equipment!E2,Variables!$A$10:$B$15,2, FALSE)*Variables!$B$7+SUM(E20:E21)*Variables!$B$6</f>
-        <v>26250</v>
+        <f>SUM(E4:E7)*Variables!$B$1 + E11*Variables!$B$4 +E8*Variables!$B$2+ SUM(Equipment!E10)*Variables!$B$3 + SUM(Equipment!E13:E15)*Variables!$B$5 + SUM(Equipment!E17:E18)* Variables!$B$6 +Equipment!E23*Variables!$B$7+ VLOOKUP(Equipment!E2,Variables!$A$12:$B$17,2, FALSE)*Variables!$B$9+SUM(E20:E21)*Variables!$B$8</f>
+        <v>22000</v>
       </c>
       <c r="F26" s="13">
-        <f>SUM(F4:F8)*Variables!$B$1 + SUM(Equipment!F10:F11)*Variables!$B$2 + SUM(Equipment!F13:F15)*Variables!$B$3 + SUM(Equipment!F17:F18)* Variables!$B$4 +Equipment!F23*Variables!$B$5+ VLOOKUP(Equipment!F2,Variables!$A$10:$B$15,2, FALSE)*Variables!$B$7+SUM(F20:F21)*Variables!$B$6</f>
-        <v>50000</v>
+        <f>SUM(F4:F7)*Variables!$B$1 + F11*Variables!$B$4 +F8*Variables!$B$2+ SUM(Equipment!F10)*Variables!$B$3 + SUM(Equipment!F13:F15)*Variables!$B$5 + SUM(Equipment!F17:F18)* Variables!$B$6 +Equipment!F23*Variables!$B$7+ VLOOKUP(Equipment!F2,Variables!$A$12:$B$17,2, FALSE)*Variables!$B$9+SUM(F20:F21)*Variables!$B$8</f>
+        <v>49200</v>
       </c>
       <c r="G26" s="13"/>
       <c r="H26" s="13">
-        <f>SUM(H4:H8)*Variables!$B$1 + SUM(Equipment!H10:H11)*Variables!$B$2 + SUM(Equipment!H13:H15)*Variables!$B$3 + SUM(Equipment!H17:H18)* Variables!$B$4 +Equipment!H23*Variables!$B$5+ VLOOKUP(Equipment!H2,Variables!$A$10:$B$15,2, FALSE)*Variables!$B$7+SUM(H20:H21)*Variables!$B$6</f>
-        <v>4147.7920040951694</v>
+        <f>SUM(H4:H7)*Variables!$B$1 + H8*Variables!$B$2+ SUM(Equipment!H10)*Variables!$B$3 + SUM(Equipment!H13:H15)*Variables!$B$5 + SUM(Equipment!H17:H18)* Variables!$B$6 +Equipment!H23*Variables!$B$7+ VLOOKUP(Equipment!H2,Variables!$A$12:$B$17,2, FALSE)*Variables!$B$9+SUM(H20:H21)*Variables!$B$8+H11*Variables!$B$4</f>
+        <v>4074.9653240882067</v>
       </c>
       <c r="I26" s="13">
-        <f>SUM(I4:I8)*Variables!$B$1 + SUM(Equipment!I10:I11)*Variables!$B$2 + SUM(Equipment!I13:I15)*Variables!$B$3 + SUM(Equipment!I17:I18)* Variables!$B$4 +Equipment!I23*Variables!$B$5+ VLOOKUP(Equipment!I2,Variables!$A$10:$B$15,2, FALSE)*Variables!$B$7+SUM(I20:I21)*Variables!$B$6</f>
-        <v>9178.4760772031004</v>
+        <f>SUM(I4:I7)*Variables!$B$1 + I8*Variables!$B$2+ SUM(Equipment!I10)*Variables!$B$3 + SUM(Equipment!I13:I15)*Variables!$B$5 + SUM(Equipment!I17:I18)* Variables!$B$6 +Equipment!I23*Variables!$B$7+ VLOOKUP(Equipment!I2,Variables!$A$12:$B$17,2, FALSE)*Variables!$B$9+SUM(I20:I21)*Variables!$B$8+I11*Variables!$B$4</f>
+        <v>11248.816132348173</v>
       </c>
       <c r="J26" s="13">
-        <f>SUM(J4:J8)*Variables!$B$1 + SUM(Equipment!J10:J11)*Variables!$B$2 + SUM(Equipment!J13:J15)*Variables!$B$3 + SUM(Equipment!J17:J18)* Variables!$B$4 +Equipment!J23*Variables!$B$5+ VLOOKUP(Equipment!J2,Variables!$A$10:$B$15,2, FALSE)*Variables!$B$7+SUM(J20:J21)*Variables!$B$6</f>
-        <v>17431.952154406201</v>
+        <f>SUM(J4:J7)*Variables!$B$1 + J8*Variables!$B$2+ SUM(Equipment!J10)*Variables!$B$3 + SUM(Equipment!J13:J15)*Variables!$B$5 + SUM(Equipment!J17:J18)* Variables!$B$6 +Equipment!J23*Variables!$B$7+ VLOOKUP(Equipment!J2,Variables!$A$12:$B$17,2, FALSE)*Variables!$B$9+SUM(J20:J21)*Variables!$B$8+J11*Variables!$B$4</f>
+        <v>22497.632264696345</v>
       </c>
       <c r="K26" s="13">
-        <f>SUM(K4:K8)*Variables!$B$1 + SUM(Equipment!K10:K11)*Variables!$B$2 + SUM(Equipment!K13:K15)*Variables!$B$3 + SUM(Equipment!K17:K18)* Variables!$B$4 +Equipment!K23*Variables!$B$5+ VLOOKUP(Equipment!K2,Variables!$A$10:$B$15,2, FALSE)*Variables!$B$7+SUM(K20:K21)*Variables!$B$6</f>
-        <v>46425.220441160578</v>
+        <f>SUM(K4:K7)*Variables!$B$1 + K8*Variables!$B$2+ SUM(Equipment!K10)*Variables!$B$3 + SUM(Equipment!K13:K15)*Variables!$B$5 + SUM(Equipment!K17:K18)* Variables!$B$6 +Equipment!K23*Variables!$B$7+ VLOOKUP(Equipment!K2,Variables!$A$12:$B$17,2, FALSE)*Variables!$B$9+SUM(K20:K21)*Variables!$B$8+K11*Variables!$B$4</f>
+        <v>43662.720441160578</v>
       </c>
       <c r="L26" s="13">
-        <f>SUM(L4:L8)*Variables!$B$1 + SUM(Equipment!L10:L11)*Variables!$B$2 + SUM(Equipment!L13:L15)*Variables!$B$3 + SUM(Equipment!L17:L18)* Variables!$B$4 +Equipment!L23*Variables!$B$5+ VLOOKUP(Equipment!L2,Variables!$A$10:$B$15,2, FALSE)*Variables!$B$7+SUM(L20:L21)*Variables!$B$6</f>
-        <v>91441.120992611279</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+        <f>SUM(L4:L7)*Variables!$B$1 + L8*Variables!$B$2+ SUM(Equipment!L10)*Variables!$B$3 + SUM(Equipment!L13:L15)*Variables!$B$5 + SUM(Equipment!L17:L18)* Variables!$B$6 +Equipment!L23*Variables!$B$7+ VLOOKUP(Equipment!L2,Variables!$A$12:$B$17,2, FALSE)*Variables!$B$9+SUM(L20:L21)*Variables!$B$8+L11*Variables!$B$4</f>
+        <v>85845.440882321156</v>
+      </c>
+      <c r="N26" s="13">
+        <f>SUM(N4:N7)*Variables!$B$1 + N8*Variables!$B$2+ SUM(Equipment!N10)*Variables!$B$3 + SUM(Equipment!N13:N15)*Variables!$B$5 + SUM(Equipment!N17:N18)* Variables!$B$6 +Equipment!N23*Variables!$B$7+ VLOOKUP(Equipment!N2,Variables!$A$12:$B$17,2, FALSE)*Variables!$B$9+SUM(N20:N21)*Variables!$B$8+N11*Variables!$B$4</f>
+        <v>1600</v>
+      </c>
+      <c r="O26" s="13">
+        <f>SUM(O4:O7)*Variables!$B$1 + O8*Variables!$B$2+ SUM(Equipment!O10)*Variables!$B$3 + SUM(Equipment!O13:O15)*Variables!$B$5 + SUM(Equipment!O17:O18)* Variables!$B$6 +Equipment!O23*Variables!$B$7+ VLOOKUP(Equipment!O2,Variables!$A$12:$B$17,2, FALSE)*Variables!$B$9+SUM(O20:O21)*Variables!$B$8+O11*Variables!$B$4</f>
+        <v>4050</v>
+      </c>
+      <c r="P26" s="13">
+        <f>SUM(P4:P7)*Variables!$B$1 + P8*Variables!$B$2+ SUM(Equipment!P10)*Variables!$B$3 + SUM(Equipment!P13:P15)*Variables!$B$5 + SUM(Equipment!P17:P18)* Variables!$B$6 +Equipment!P23*Variables!$B$7+ VLOOKUP(Equipment!P2,Variables!$A$12:$B$17,2, FALSE)*Variables!$B$9+SUM(P20:P21)*Variables!$B$8+P11*Variables!$B$4</f>
+        <v>10500</v>
+      </c>
+      <c r="Q26" s="13">
+        <f>SUM(Q4:Q7)*Variables!$B$1 + Q8*Variables!$B$2+ SUM(Equipment!Q10)*Variables!$B$3 + SUM(Equipment!Q13:Q15)*Variables!$B$5 + SUM(Equipment!Q17:Q18)* Variables!$B$6 +Equipment!Q23*Variables!$B$7+ VLOOKUP(Equipment!Q2,Variables!$A$12:$B$17,2, FALSE)*Variables!$B$9+SUM(Q20:Q21)*Variables!$B$8+Q11*Variables!$B$4</f>
+        <v>20000</v>
+      </c>
+      <c r="R26" s="13">
+        <f>SUM(R4:R7)*Variables!$B$1 + R8*Variables!$B$2+ SUM(Equipment!R10)*Variables!$B$3 + SUM(Equipment!R13:R15)*Variables!$B$5 + SUM(Equipment!R17:R18)* Variables!$B$6 +Equipment!R23*Variables!$B$7+ VLOOKUP(Equipment!R2,Variables!$A$12:$B$17,2, FALSE)*Variables!$B$9+SUM(R20:R21)*Variables!$B$8+R11*Variables!$B$4</f>
+        <v>45900</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="12">
-        <f>B26*VLOOKUP(Equipment!B2,Variables!$A$10:$C$15,3,FALSE)</f>
+        <f>VLOOKUP(Equipment!B2,Variables!$A$12:$D$17,4,FALSE)</f>
         <v>2000</v>
       </c>
       <c r="C27" s="12">
-        <f>B27*VLOOKUP(Equipment!C2,Variables!$A$10:$C$15,3,FALSE)</f>
+        <f>B27*VLOOKUP(Equipment!C2,Variables!$A$12:$C$17,3,FALSE)</f>
         <v>5000</v>
       </c>
       <c r="D27" s="12">
-        <f>C27*VLOOKUP(Equipment!D2,Variables!$A$10:$C$15,3,FALSE)</f>
+        <f>C27*VLOOKUP(Equipment!D2,Variables!$A$12:$C$17,3,FALSE)</f>
         <v>10000</v>
       </c>
       <c r="E27" s="12">
-        <f>D27*VLOOKUP(Equipment!E2,Variables!$A$10:$C$15,3,FALSE)</f>
+        <f>D27*VLOOKUP(Equipment!E2,Variables!$A$12:$C$17,3,FALSE)</f>
         <v>25000</v>
       </c>
       <c r="F27" s="12">
-        <f>E27*VLOOKUP(Equipment!F2,Variables!$A$10:$C$15,3,FALSE)</f>
+        <f>E27*VLOOKUP(Equipment!F2,Variables!$A$12:$C$17,3,FALSE)</f>
         <v>50000</v>
       </c>
       <c r="G27" s="12"/>
       <c r="H27" s="12">
-        <f>H26*VLOOKUP(Equipment!H2,Variables!$A$10:$C$15,3,FALSE)</f>
-        <v>4147.7920040951694</v>
+        <f>H26*VLOOKUP(Equipment!H2,Variables!$A$12:$C$17,3,FALSE)</f>
+        <v>4074.9653240882067</v>
       </c>
       <c r="I27" s="12">
-        <f>H27*VLOOKUP(Equipment!I2,Variables!$A$10:$C$15,3,FALSE)</f>
-        <v>10369.480010237923</v>
+        <f>H27*VLOOKUP(Equipment!I2,Variables!$A$12:$C$17,3,FALSE)</f>
+        <v>10187.413310220516</v>
       </c>
       <c r="J27" s="12">
-        <f>I27*VLOOKUP(Equipment!J2,Variables!$A$10:$C$15,3,FALSE)</f>
-        <v>20738.960020475846</v>
+        <f>I27*VLOOKUP(Equipment!J2,Variables!$A$12:$C$17,3,FALSE)</f>
+        <v>20374.826620441032</v>
       </c>
       <c r="K27" s="12">
-        <f>J27*VLOOKUP(Equipment!K2,Variables!$A$10:$C$15,3,FALSE)</f>
-        <v>51847.400051189616</v>
+        <f>J27*VLOOKUP(Equipment!K2,Variables!$A$12:$C$17,3,FALSE)</f>
+        <v>50937.06655110258</v>
       </c>
       <c r="L27" s="12">
-        <f>K27*VLOOKUP(Equipment!L2,Variables!$A$10:$C$15,3,FALSE)</f>
-        <v>103694.80010237923</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <f>K27*VLOOKUP(Equipment!L2,Variables!$A$12:$C$17,3,FALSE)</f>
+        <v>101874.13310220516</v>
+      </c>
+      <c r="N27" s="12">
+        <f>N26*VLOOKUP(Equipment!N2,Variables!$A$12:$C$17,3,FALSE)</f>
+        <v>1600</v>
+      </c>
+      <c r="O27" s="12">
+        <f>N27*VLOOKUP(Equipment!O2,Variables!$A$12:$C$17,3,FALSE)</f>
+        <v>4000</v>
+      </c>
+      <c r="P27" s="12">
+        <f>O27*VLOOKUP(Equipment!P2,Variables!$A$12:$C$17,3,FALSE)</f>
+        <v>8000</v>
+      </c>
+      <c r="Q27" s="12">
+        <f>P27*VLOOKUP(Equipment!Q2,Variables!$A$12:$C$17,3,FALSE)</f>
+        <v>20000</v>
+      </c>
+      <c r="R27" s="12">
+        <f>Q27*VLOOKUP(Equipment!R2,Variables!$A$12:$C$17,3,FALSE)</f>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" s="13">
         <f>B27-B26</f>
@@ -1734,7 +2173,7 @@
       </c>
       <c r="C28" s="13">
         <f t="shared" ref="C28:F28" si="0">C27-C26</f>
-        <v>-250</v>
+        <v>0</v>
       </c>
       <c r="D28" s="13">
         <f t="shared" si="0"/>
@@ -1742,11 +2181,11 @@
       </c>
       <c r="E28" s="13">
         <f t="shared" si="0"/>
-        <v>-1250</v>
+        <v>3000</v>
       </c>
       <c r="F28" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="G28" s="13"/>
       <c r="H28" s="13">
@@ -1755,112 +2194,213 @@
       </c>
       <c r="I28" s="13">
         <f t="shared" ref="I28" si="1">I27-I26</f>
-        <v>1191.0039330348227</v>
+        <v>-1061.4028221276567</v>
       </c>
       <c r="J28" s="13">
         <f t="shared" ref="J28" si="2">J27-J26</f>
-        <v>3307.0078660696454</v>
+        <v>-2122.8056442553134</v>
       </c>
       <c r="K28" s="13">
         <f t="shared" ref="K28" si="3">K27-K26</f>
-        <v>5422.1796100290376</v>
+        <v>7274.3461099420019</v>
       </c>
       <c r="L28" s="13">
         <f t="shared" ref="L28" si="4">L27-L26</f>
-        <v>12253.679109767952</v>
+        <v>16028.692219884004</v>
+      </c>
+      <c r="N28" s="13">
+        <f>N27-N26</f>
+        <v>0</v>
+      </c>
+      <c r="O28" s="13">
+        <f t="shared" ref="O28:R28" si="5">O27-O26</f>
+        <v>-50</v>
+      </c>
+      <c r="P28" s="13">
+        <f t="shared" si="5"/>
+        <v>-2500</v>
+      </c>
+      <c r="Q28" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R28" s="13">
+        <f t="shared" si="5"/>
+        <v>-5900</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="H1:L1"/>
+    <mergeCell ref="N1:R1"/>
   </mergeCells>
-  <conditionalFormatting sqref="M2:XFD2 A2:C2">
-    <cfRule type="containsText" dxfId="44" priority="45" operator="containsText" text="Relic">
+  <conditionalFormatting sqref="M2 A2:C2 S2:XFD2">
+    <cfRule type="containsText" dxfId="64" priority="66" operator="containsText" text="Relic">
       <formula>NOT(ISERROR(SEARCH("Relic",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="46" operator="containsText" text="Legendary">
+    <cfRule type="containsText" dxfId="63" priority="67" operator="containsText" text="Legendary">
       <formula>NOT(ISERROR(SEARCH("Legendary",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="47" operator="containsText" text="Epic">
+    <cfRule type="containsText" dxfId="62" priority="68" operator="containsText" text="Epic">
       <formula>NOT(ISERROR(SEARCH("Epic",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="48" operator="containsText" text="Rare">
+    <cfRule type="containsText" dxfId="61" priority="69" operator="containsText" text="Rare">
       <formula>NOT(ISERROR(SEARCH("Rare",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="49" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="60" priority="70" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="39" priority="40" operator="containsText" text="Relic">
+    <cfRule type="containsText" dxfId="59" priority="61" operator="containsText" text="Relic">
       <formula>NOT(ISERROR(SEARCH("Relic",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="41" operator="containsText" text="Legendary">
+    <cfRule type="containsText" dxfId="58" priority="62" operator="containsText" text="Legendary">
       <formula>NOT(ISERROR(SEARCH("Legendary",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="42" operator="containsText" text="Epic">
+    <cfRule type="containsText" dxfId="57" priority="63" operator="containsText" text="Epic">
       <formula>NOT(ISERROR(SEARCH("Epic",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="43" operator="containsText" text="Rare">
+    <cfRule type="containsText" dxfId="56" priority="64" operator="containsText" text="Rare">
       <formula>NOT(ISERROR(SEARCH("Rare",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="44" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="55" priority="65" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="Relic">
+    <cfRule type="containsText" dxfId="54" priority="56" operator="containsText" text="Relic">
       <formula>NOT(ISERROR(SEARCH("Relic",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="Legendary">
+    <cfRule type="containsText" dxfId="53" priority="57" operator="containsText" text="Legendary">
       <formula>NOT(ISERROR(SEARCH("Legendary",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="37" operator="containsText" text="Epic">
+    <cfRule type="containsText" dxfId="52" priority="58" operator="containsText" text="Epic">
       <formula>NOT(ISERROR(SEARCH("Epic",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="38" operator="containsText" text="Rare">
+    <cfRule type="containsText" dxfId="51" priority="59" operator="containsText" text="Rare">
       <formula>NOT(ISERROR(SEARCH("Rare",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="39" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="50" priority="60" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="containsText" dxfId="29" priority="30" operator="containsText" text="Relic">
+    <cfRule type="containsText" dxfId="49" priority="51" operator="containsText" text="Relic">
       <formula>NOT(ISERROR(SEARCH("Relic",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="31" operator="containsText" text="Legendary">
+    <cfRule type="containsText" dxfId="48" priority="52" operator="containsText" text="Legendary">
       <formula>NOT(ISERROR(SEARCH("Legendary",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="32" operator="containsText" text="Epic">
+    <cfRule type="containsText" dxfId="47" priority="53" operator="containsText" text="Epic">
       <formula>NOT(ISERROR(SEARCH("Epic",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="33" operator="containsText" text="Rare">
+    <cfRule type="containsText" dxfId="46" priority="54" operator="containsText" text="Rare">
       <formula>NOT(ISERROR(SEARCH("Rare",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="34" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="45" priority="55" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2">
-    <cfRule type="containsText" dxfId="24" priority="25" operator="containsText" text="Relic">
+    <cfRule type="containsText" dxfId="44" priority="46" operator="containsText" text="Relic">
       <formula>NOT(ISERROR(SEARCH("Relic",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="26" operator="containsText" text="Legendary">
+    <cfRule type="containsText" dxfId="43" priority="47" operator="containsText" text="Legendary">
       <formula>NOT(ISERROR(SEARCH("Legendary",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="27" operator="containsText" text="Epic">
+    <cfRule type="containsText" dxfId="42" priority="48" operator="containsText" text="Epic">
       <formula>NOT(ISERROR(SEARCH("Epic",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="28" operator="containsText" text="Rare">
+    <cfRule type="containsText" dxfId="41" priority="49" operator="containsText" text="Rare">
       <formula>NOT(ISERROR(SEARCH("Rare",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="29" operator="containsText" text="Uncommon">
+    <cfRule type="containsText" dxfId="40" priority="50" operator="containsText" text="Uncommon">
       <formula>NOT(ISERROR(SEARCH("Uncommon",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28:G28">
+  <conditionalFormatting sqref="B28:G28">
+    <cfRule type="colorScale" priority="43">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:I2">
+    <cfRule type="containsText" dxfId="39" priority="38" operator="containsText" text="Relic">
+      <formula>NOT(ISERROR(SEARCH("Relic",H2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="38" priority="39" operator="containsText" text="Legendary">
+      <formula>NOT(ISERROR(SEARCH("Legendary",H2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="40" operator="containsText" text="Epic">
+      <formula>NOT(ISERROR(SEARCH("Epic",H2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="41" operator="containsText" text="Rare">
+      <formula>NOT(ISERROR(SEARCH("Rare",H2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="35" priority="42" operator="containsText" text="Uncommon">
+      <formula>NOT(ISERROR(SEARCH("Uncommon",H2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2">
+    <cfRule type="containsText" dxfId="34" priority="33" operator="containsText" text="Relic">
+      <formula>NOT(ISERROR(SEARCH("Relic",J2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="33" priority="34" operator="containsText" text="Legendary">
+      <formula>NOT(ISERROR(SEARCH("Legendary",J2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="32" priority="35" operator="containsText" text="Epic">
+      <formula>NOT(ISERROR(SEARCH("Epic",J2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="36" operator="containsText" text="Rare">
+      <formula>NOT(ISERROR(SEARCH("Rare",J2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="37" operator="containsText" text="Uncommon">
+      <formula>NOT(ISERROR(SEARCH("Uncommon",J2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2">
+    <cfRule type="containsText" dxfId="29" priority="28" operator="containsText" text="Relic">
+      <formula>NOT(ISERROR(SEARCH("Relic",K2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="Legendary">
+      <formula>NOT(ISERROR(SEARCH("Legendary",K2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="27" priority="30" operator="containsText" text="Epic">
+      <formula>NOT(ISERROR(SEARCH("Epic",K2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="31" operator="containsText" text="Rare">
+      <formula>NOT(ISERROR(SEARCH("Rare",K2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="32" operator="containsText" text="Uncommon">
+      <formula>NOT(ISERROR(SEARCH("Uncommon",K2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2">
+    <cfRule type="containsText" dxfId="24" priority="23" operator="containsText" text="Relic">
+      <formula>NOT(ISERROR(SEARCH("Relic",L2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="23" priority="24" operator="containsText" text="Legendary">
+      <formula>NOT(ISERROR(SEARCH("Legendary",L2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="25" operator="containsText" text="Epic">
+      <formula>NOT(ISERROR(SEARCH("Epic",L2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="26" operator="containsText" text="Rare">
+      <formula>NOT(ISERROR(SEARCH("Rare",L2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="27" operator="containsText" text="Uncommon">
+      <formula>NOT(ISERROR(SEARCH("Uncommon",L2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I28:L28">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -1872,75 +2412,75 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:I2">
+  <conditionalFormatting sqref="N2:O2">
     <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="Relic">
-      <formula>NOT(ISERROR(SEARCH("Relic",H2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Relic",N2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="Legendary">
-      <formula>NOT(ISERROR(SEARCH("Legendary",H2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Legendary",N2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="Epic">
-      <formula>NOT(ISERROR(SEARCH("Epic",H2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Epic",N2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="Rare">
-      <formula>NOT(ISERROR(SEARCH("Rare",H2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Rare",N2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="15" priority="21" operator="containsText" text="Uncommon">
-      <formula>NOT(ISERROR(SEARCH("Uncommon",H2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Uncommon",N2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2">
+  <conditionalFormatting sqref="P2">
     <cfRule type="containsText" dxfId="14" priority="12" operator="containsText" text="Relic">
-      <formula>NOT(ISERROR(SEARCH("Relic",J2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Relic",P2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="Legendary">
-      <formula>NOT(ISERROR(SEARCH("Legendary",J2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Legendary",P2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="Epic">
-      <formula>NOT(ISERROR(SEARCH("Epic",J2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Epic",P2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="11" priority="15" operator="containsText" text="Rare">
-      <formula>NOT(ISERROR(SEARCH("Rare",J2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Rare",P2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="10" priority="16" operator="containsText" text="Uncommon">
-      <formula>NOT(ISERROR(SEARCH("Uncommon",J2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Uncommon",P2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2">
+  <conditionalFormatting sqref="Q2">
     <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="Relic">
-      <formula>NOT(ISERROR(SEARCH("Relic",K2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Relic",Q2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="Legendary">
-      <formula>NOT(ISERROR(SEARCH("Legendary",K2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Legendary",Q2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="Epic">
-      <formula>NOT(ISERROR(SEARCH("Epic",K2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Epic",Q2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="Rare">
-      <formula>NOT(ISERROR(SEARCH("Rare",K2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Rare",Q2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="5" priority="11" operator="containsText" text="Uncommon">
-      <formula>NOT(ISERROR(SEARCH("Uncommon",K2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Uncommon",Q2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2">
+  <conditionalFormatting sqref="R2">
     <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Relic">
-      <formula>NOT(ISERROR(SEARCH("Relic",L2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Relic",R2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Legendary">
-      <formula>NOT(ISERROR(SEARCH("Legendary",L2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Legendary",R2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Epic">
-      <formula>NOT(ISERROR(SEARCH("Epic",L2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Epic",R2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Rare">
-      <formula>NOT(ISERROR(SEARCH("Rare",L2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Rare",R2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="Uncommon">
-      <formula>NOT(ISERROR(SEARCH("Uncommon",L2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Uncommon",R2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I28:L28">
+  <conditionalFormatting sqref="O28:R28">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1958,9 +2498,9 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CECBE0D3-5D4B-4C36-81F6-E7FEB94B352D}">
           <x14:formula1>
-            <xm:f>Variables!$A$10:$A$15</xm:f>
+            <xm:f>Variables!$A$12:$A$17</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:L2</xm:sqref>
+          <xm:sqref>B2:L2 N2:R2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1970,10 +2510,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633D427C-AAB3-42F7-80CE-7F014982D833}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1988,174 +2528,194 @@
         <v>18</v>
       </c>
       <c r="B1">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="B3">
-        <v>50</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="B4">
-        <v>-100000</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B5">
-        <v>5000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="B6">
-        <v>100000</v>
+        <v>-200000</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B7">
+      <c r="B11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" s="10">
         <v>2000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" s="10">
-        <v>2020</v>
-      </c>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>2.5</v>
-      </c>
-      <c r="D11" s="10">
-        <f>C11*D10</f>
-        <v>5050</v>
-      </c>
-      <c r="E11" s="9"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12" s="10">
-        <f t="shared" ref="D12:D14" si="0">C12*D11</f>
-        <v>10100</v>
       </c>
       <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <v>2.5</v>
       </c>
       <c r="D13" s="10">
-        <f t="shared" si="0"/>
-        <v>25250</v>
+        <f>C13*D12</f>
+        <v>5000</v>
       </c>
       <c r="E13" s="9"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
       <c r="D14" s="10">
+        <f t="shared" ref="D14:D16" si="0">C14*D13</f>
+        <v>10000</v>
+      </c>
+      <c r="E14" s="9"/>
+    </row>
+    <row r="15" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>2.5</v>
+      </c>
+      <c r="D15" s="10">
         <f t="shared" si="0"/>
-        <v>50500</v>
-      </c>
-      <c r="E14" s="9"/>
-    </row>
-    <row r="15" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="D15" s="17"/>
+        <v>25000</v>
+      </c>
       <c r="E15" s="18"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
+      <c r="A16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" s="10">
+        <f t="shared" si="0"/>
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="16"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="17"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18">
+      <c r="B20">
         <v>1.85</v>
       </c>
     </row>
@@ -2192,23 +2752,23 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="23"/>
     </row>
@@ -2217,7 +2777,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2228,10 +2788,10 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="21" t="s">
         <v>42</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2242,7 +2802,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" s="19">
         <v>-0.05</v>

</xml_diff>